<commit_message>
Data Driven Framework - Part 2
</commit_message>
<xml_diff>
--- a/src/test/resources/TutorialsNinja.xlsx
+++ b/src/test/resources/TutorialsNinja.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QAFox\BatchOne\DataDrivenFrameworkWorkspace\DDFProj\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAFA54F-FD58-4789-A562-B1BC3644456C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7E270F-9E2F-44FF-BC52-2E61283DEE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>TestCase</t>
   </si>
@@ -160,7 +160,10 @@
     <t>ExpectedProduct</t>
   </si>
   <si>
-    <t>No Product</t>
+    <t>HP LP3065</t>
+  </si>
+  <si>
+    <t>There is no product that matches the search criteria.</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -291,39 +294,24 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -359,13 +347,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -651,7 +639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -687,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -700,16 +690,16 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -823,7 +813,7 @@
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>12</v>
@@ -881,7 +871,7 @@
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>12</v>
@@ -913,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>34</v>
@@ -942,72 +932,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="14" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Driven Framework Improvisation - Part 1
</commit_message>
<xml_diff>
--- a/src/test/resources/TutorialsNinja.xlsx
+++ b/src/test/resources/TutorialsNinja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QAFox\BatchOne\DataDrivenFrameworkWorkspace\DDFProj\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7E270F-9E2F-44FF-BC52-2E61283DEE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A627673-ED84-42E3-89F9-C004C5F2F960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>TestCase</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Runmode</t>
@@ -639,9 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -653,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -669,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,19 +706,19 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -731,16 +726,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -748,16 +743,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -765,16 +760,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -784,31 +779,31 @@
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="C8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -816,28 +811,28 @@
         <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="F9" s="8">
         <v>1234567890</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -845,28 +840,28 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="E10" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="10">
         <v>1234567891</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -874,28 +869,28 @@
         <v>4</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="E11" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="10">
         <v>1234567892</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -903,28 +898,28 @@
         <v>4</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="10">
         <v>1234567893</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -934,19 +929,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>7</v>
-      </c>
       <c r="C15" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -954,16 +949,16 @@
         <v>4</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -971,16 +966,16 @@
         <v>4</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -988,16 +983,16 @@
         <v>4</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Driven Framework Improvisation - Part 2
</commit_message>
<xml_diff>
--- a/src/test/resources/TutorialsNinja.xlsx
+++ b/src/test/resources/TutorialsNinja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QAFox\BatchOne\DataDrivenFrameworkWorkspace\DDFProj\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A627673-ED84-42E3-89F9-C004C5F2F960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D344A5-339E-4388-B6B5-0E93F0EBD3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testcases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>TestCase</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>There is no product that matches the search criteria.</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -684,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CD3E39-C002-4FB9-9141-BDBB459D862D}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -837,7 +840,7 @@
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>10</v>

</xml_diff>